<commit_message>
Changes for version 2.0, fixed database is locked error and reorganized app
</commit_message>
<xml_diff>
--- a/Data/Excel/2018/vaseis1.xlsx
+++ b/Data/Excel/2018/vaseis1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\My Projects\ypologismosMorion\Data\Excel\2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F9617D-4EE9-4321-B104-A0B4A9D98859}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47437F18-9681-4A55-B6EC-18985123ECC7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{167C75AF-3B4F-4B99-914F-A3A93AB81AB5}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="176">
   <si>
     <t>ΑΕΙ</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>poli</t>
+  </si>
+  <si>
+    <t>existsinNewest</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,10 @@
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -656,13 +662,14 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{6FE89AF6-237A-4EA8-9A06-8F11A657620A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="19" unboundColumnsRight="7">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="20" unboundColumnsRight="8">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Α/Α, Κωδικός Μηχανογραφικού" tableColumnId="1"/>
       <queryTableField id="2" dataBound="0" tableColumnId="2"/>
       <queryTableField id="3" dataBound="0" tableColumnId="3"/>
       <queryTableField id="4" dataBound="0" tableColumnId="4"/>
       <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="19" dataBound="0" tableColumnId="6"/>
       <queryTableField id="16" dataBound="0" tableColumnId="16"/>
       <queryTableField id="17" dataBound="0" tableColumnId="17"/>
       <queryTableField id="18" dataBound="0" tableColumnId="18"/>
@@ -688,14 +695,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C388DD16-8B19-4B76-B83C-C0389824C7D5}" name="για_αποφοίτους_90____ΓΕΛ___ΗΜΕΡΗΣΙΑ" displayName="για_αποφοίτους_90____ΓΕΛ___ΗΜΕΡΗΣΙΑ" ref="A1:H1048576" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H1048576" xr:uid="{DCED3EF1-ECB3-4DF5-BC22-780C2865EE38}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{69CCEBD1-4FBE-448C-A00D-BE93F7696DD7}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{61EDBF58-8FEF-4CF6-B062-833F777FE71D}" uniqueName="2" name="Mixanografiko" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{D22AF6F6-437F-4A6B-A1C6-592A44A358F5}" uniqueName="3" name="idryma" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A330B982-354D-4FD0-AFD4-8051EEF06523}" uniqueName="4" name="sxoli" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{C74F8C2A-4D2D-4F6B-BCD5-4F0C2F578F09}" uniqueName="5" name="eidika" queryTableFieldId="5" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C388DD16-8B19-4B76-B83C-C0389824C7D5}" name="για_αποφοίτους_90____ΓΕΛ___ΗΜΕΡΗΣΙΑ" displayName="για_αποφοίτους_90____ΓΕΛ___ΗΜΕΡΗΣΙΑ" ref="A1:I1048576" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I1048576" xr:uid="{DCED3EF1-ECB3-4DF5-BC22-780C2865EE38}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{69CCEBD1-4FBE-448C-A00D-BE93F7696DD7}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{61EDBF58-8FEF-4CF6-B062-833F777FE71D}" uniqueName="2" name="Mixanografiko" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D22AF6F6-437F-4A6B-A1C6-592A44A358F5}" uniqueName="3" name="idryma" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A330B982-354D-4FD0-AFD4-8051EEF06523}" uniqueName="4" name="sxoli" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C74F8C2A-4D2D-4F6B-BCD5-4F0C2F578F09}" uniqueName="5" name="eidika" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{0F130DC8-45B8-4AE0-9A6F-6EC21592E744}" uniqueName="6" name="existsinNewest" queryTableFieldId="19" dataDxfId="3"/>
     <tableColumn id="16" xr3:uid="{E7943A49-C5AD-469B-BEB2-549AFCE44A5E}" uniqueName="16" name="typos" queryTableFieldId="16" dataDxfId="2"/>
     <tableColumn id="17" xr3:uid="{1927F29C-81FB-4085-9EBE-CF8B37E473D0}" uniqueName="17" name="poli" queryTableFieldId="17" dataDxfId="1"/>
     <tableColumn id="18" xr3:uid="{55B5BB7A-4E1E-4803-8039-561E1C092A20}" uniqueName="18" name="vasi" queryTableFieldId="18" dataDxfId="0"/>
@@ -1001,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B52A64-D77D-46EE-9008-CE7B2B84E66F}">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,12 +1022,13 @@
     <col min="3" max="3" width="58.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="70.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.21875" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1036,16 +1045,19 @@
         <v>172</v>
       </c>
       <c r="F1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" t="s">
         <v>173</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>174</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1061,17 +1073,18 @@
       <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F2"/>
       <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>20039</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1087,17 +1100,18 @@
       <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F3"/>
       <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>19708</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>112</v>
       </c>
@@ -1113,17 +1127,18 @@
       <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4"/>
+      <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>18881</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>113</v>
       </c>
@@ -1139,17 +1154,18 @@
       <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5"/>
+      <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>18844</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -1165,17 +1181,18 @@
       <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F6"/>
       <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>18578</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>123</v>
       </c>
@@ -1191,17 +1208,18 @@
       <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7"/>
+      <c r="G7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>18395</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>68</v>
       </c>
@@ -1215,17 +1233,18 @@
         <v>48</v>
       </c>
       <c r="E8"/>
-      <c r="F8" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F8"/>
       <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>18219</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>16</v>
       </c>
@@ -1241,17 +1260,18 @@
       <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F9"/>
       <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>18141</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>120</v>
       </c>
@@ -1267,17 +1287,18 @@
       <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10"/>
+      <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>18123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>69</v>
       </c>
@@ -1291,17 +1312,18 @@
         <v>48</v>
       </c>
       <c r="E11"/>
-      <c r="F11" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F11"/>
       <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>17965</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>108</v>
       </c>
@@ -1315,17 +1337,18 @@
         <v>53</v>
       </c>
       <c r="E12"/>
-      <c r="F12" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F12"/>
       <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>17949</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>22</v>
       </c>
@@ -1341,17 +1364,18 @@
       <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F13"/>
       <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>17924</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>110</v>
       </c>
@@ -1365,17 +1389,18 @@
         <v>53</v>
       </c>
       <c r="E14"/>
-      <c r="F14" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F14"/>
       <c r="G14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>17711</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>23</v>
       </c>
@@ -1391,17 +1416,18 @@
       <c r="E15" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F15"/>
       <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>17588</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>109</v>
       </c>
@@ -1415,17 +1441,18 @@
         <v>53</v>
       </c>
       <c r="E16"/>
-      <c r="F16" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F16"/>
       <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>17579</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>122</v>
       </c>
@@ -1441,17 +1468,18 @@
       <c r="E17" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17"/>
+      <c r="G17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>17518</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>70</v>
       </c>
@@ -1465,17 +1493,18 @@
         <v>48</v>
       </c>
       <c r="E18"/>
-      <c r="F18" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F18"/>
       <c r="G18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>17465</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>20</v>
       </c>
@@ -1491,17 +1520,18 @@
       <c r="E19" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F19"/>
       <c r="G19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>17426</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>111</v>
       </c>
@@ -1515,17 +1545,18 @@
         <v>53</v>
       </c>
       <c r="E20"/>
-      <c r="F20" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F20"/>
       <c r="G20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>17341</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>71</v>
       </c>
@@ -1541,17 +1572,18 @@
       <c r="E21" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F21"/>
       <c r="G21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>17317</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>124</v>
       </c>
@@ -1567,17 +1599,18 @@
       <c r="E22" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22"/>
+      <c r="G22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>17264</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>64</v>
       </c>
@@ -1593,17 +1626,18 @@
       <c r="E23" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F23"/>
       <c r="G23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>17028</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>13</v>
       </c>
@@ -1619,17 +1653,18 @@
       <c r="E24" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F24"/>
       <c r="G24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>16799</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1645,17 +1680,18 @@
       <c r="E25" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F25"/>
       <c r="G25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>16719</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>18</v>
       </c>
@@ -1669,17 +1705,18 @@
         <v>69</v>
       </c>
       <c r="E26"/>
-      <c r="F26" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F26"/>
       <c r="G26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>16711</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>121</v>
       </c>
@@ -1695,17 +1732,18 @@
       <c r="E27" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27"/>
+      <c r="G27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>16695</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>87</v>
       </c>
@@ -1719,17 +1757,18 @@
         <v>71</v>
       </c>
       <c r="E28"/>
-      <c r="F28" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F28"/>
       <c r="G28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>16658</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1745,17 +1784,18 @@
       <c r="E29" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F29"/>
       <c r="G29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>16372</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>91</v>
       </c>
@@ -1769,17 +1809,18 @@
         <v>73</v>
       </c>
       <c r="E30"/>
-      <c r="F30" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F30"/>
       <c r="G30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>16370</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>55</v>
       </c>
@@ -1793,17 +1834,18 @@
         <v>75</v>
       </c>
       <c r="E31"/>
-      <c r="F31" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F31"/>
       <c r="G31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>16284</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>96</v>
       </c>
@@ -1817,17 +1859,18 @@
         <v>76</v>
       </c>
       <c r="E32"/>
-      <c r="F32" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F32"/>
       <c r="G32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>16267</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>40</v>
       </c>
@@ -1841,17 +1884,18 @@
         <v>77</v>
       </c>
       <c r="E33"/>
-      <c r="F33" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F33"/>
       <c r="G33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>16231</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>81</v>
       </c>
@@ -1865,17 +1909,18 @@
         <v>78</v>
       </c>
       <c r="E34"/>
-      <c r="F34" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F34"/>
       <c r="G34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>16175</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>72</v>
       </c>
@@ -1889,17 +1934,18 @@
         <v>79</v>
       </c>
       <c r="E35"/>
-      <c r="F35" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F35"/>
       <c r="G35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>16059</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>97</v>
       </c>
@@ -1913,17 +1959,18 @@
         <v>76</v>
       </c>
       <c r="E36"/>
-      <c r="F36" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F36"/>
       <c r="G36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>15863</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>41</v>
       </c>
@@ -1937,17 +1984,18 @@
         <v>77</v>
       </c>
       <c r="E37"/>
-      <c r="F37" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F37"/>
       <c r="G37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>15853</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>25</v>
       </c>
@@ -1963,17 +2011,18 @@
       <c r="E38" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F38"/>
       <c r="G38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>15825</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>88</v>
       </c>
@@ -1987,17 +2036,18 @@
         <v>80</v>
       </c>
       <c r="E39"/>
-      <c r="F39" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F39"/>
       <c r="G39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>15722</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>60</v>
       </c>
@@ -2011,17 +2061,18 @@
         <v>81</v>
       </c>
       <c r="E40"/>
-      <c r="F40" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F40"/>
       <c r="G40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>15722</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>75</v>
       </c>
@@ -2035,17 +2086,18 @@
         <v>79</v>
       </c>
       <c r="E41"/>
-      <c r="F41" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F41"/>
       <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>15473</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>24</v>
       </c>
@@ -2061,17 +2113,18 @@
       <c r="E42" t="s">
         <v>55</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F42"/>
       <c r="G42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>15352</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>102</v>
       </c>
@@ -2084,20 +2137,20 @@
       <c r="D43" t="s">
         <v>82</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <v>15350</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>17</v>
       </c>
@@ -2111,17 +2164,18 @@
         <v>84</v>
       </c>
       <c r="E44"/>
-      <c r="F44" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F44"/>
       <c r="G44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>15340</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>6</v>
       </c>
@@ -2135,17 +2189,18 @@
         <v>85</v>
       </c>
       <c r="E45"/>
-      <c r="F45" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F45"/>
       <c r="G45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <v>15216</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>12</v>
       </c>
@@ -2159,17 +2214,18 @@
         <v>86</v>
       </c>
       <c r="E46"/>
-      <c r="F46" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F46"/>
       <c r="G46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <v>15117</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>66</v>
       </c>
@@ -2185,17 +2241,18 @@
       <c r="E47" t="s">
         <v>88</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F47"/>
       <c r="G47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <v>15095</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>93</v>
       </c>
@@ -2209,17 +2266,18 @@
         <v>89</v>
       </c>
       <c r="E48"/>
-      <c r="F48" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F48"/>
       <c r="G48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H48" s="1">
+      <c r="I48" s="1">
         <v>14925</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>54</v>
       </c>
@@ -2233,17 +2291,18 @@
         <v>90</v>
       </c>
       <c r="E49"/>
-      <c r="F49" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F49"/>
       <c r="G49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>14867</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>104</v>
       </c>
@@ -2257,17 +2316,18 @@
         <v>91</v>
       </c>
       <c r="E50"/>
-      <c r="F50" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F50"/>
       <c r="G50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H50" s="1">
+      <c r="I50" s="1">
         <v>14748</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>77</v>
       </c>
@@ -2280,20 +2340,20 @@
       <c r="D51" t="s">
         <v>79</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>83</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="1">
+      <c r="I51" s="1">
         <v>14748</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>128</v>
       </c>
@@ -2306,20 +2366,20 @@
       <c r="D52" t="s">
         <v>75</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>83</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="1">
+      <c r="I52" s="1">
         <v>14698</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>27</v>
       </c>
@@ -2333,17 +2393,18 @@
         <v>93</v>
       </c>
       <c r="E53"/>
-      <c r="F53" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F53"/>
       <c r="G53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H53" s="1">
+      <c r="I53" s="1">
         <v>14674</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>74</v>
       </c>
@@ -2357,17 +2418,18 @@
         <v>79</v>
       </c>
       <c r="E54"/>
-      <c r="F54" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F54"/>
       <c r="G54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="1">
+      <c r="I54" s="1">
         <v>14647</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>59</v>
       </c>
@@ -2381,17 +2443,18 @@
         <v>94</v>
       </c>
       <c r="E55"/>
-      <c r="F55" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F55"/>
       <c r="G55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="1">
+      <c r="I55" s="1">
         <v>14553</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>90</v>
       </c>
@@ -2405,17 +2468,18 @@
         <v>96</v>
       </c>
       <c r="E56"/>
-      <c r="F56" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F56"/>
       <c r="G56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H56" s="1">
+      <c r="I56" s="1">
         <v>14423</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -2429,17 +2493,18 @@
         <v>97</v>
       </c>
       <c r="E57"/>
-      <c r="F57" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F57"/>
       <c r="G57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H57" s="1">
+      <c r="I57" s="1">
         <v>14273</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>76</v>
       </c>
@@ -2453,17 +2518,18 @@
         <v>79</v>
       </c>
       <c r="E58"/>
-      <c r="F58" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F58"/>
       <c r="G58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H58" s="1">
+      <c r="I58" s="1">
         <v>14267</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>100</v>
       </c>
@@ -2477,17 +2543,18 @@
         <v>76</v>
       </c>
       <c r="E59"/>
-      <c r="F59" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F59"/>
       <c r="G59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="1">
+      <c r="I59" s="1">
         <v>14185</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>34</v>
       </c>
@@ -2501,17 +2568,18 @@
         <v>99</v>
       </c>
       <c r="E60"/>
-      <c r="F60" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F60"/>
       <c r="G60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H60" s="1">
+      <c r="I60" s="1">
         <v>14105</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>48</v>
       </c>
@@ -2525,17 +2593,18 @@
         <v>100</v>
       </c>
       <c r="E61"/>
-      <c r="F61" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F61"/>
       <c r="G61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="1">
+      <c r="I61" s="1">
         <v>14058</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>51</v>
       </c>
@@ -2549,17 +2618,18 @@
         <v>101</v>
       </c>
       <c r="E62"/>
-      <c r="F62" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F62"/>
       <c r="G62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H62" s="1">
+      <c r="I62" s="1">
         <v>13847</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>45</v>
       </c>
@@ -2573,17 +2643,18 @@
         <v>102</v>
       </c>
       <c r="E63"/>
-      <c r="F63" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F63"/>
       <c r="G63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H63" s="1">
+      <c r="I63" s="1">
         <v>13841</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>78</v>
       </c>
@@ -2597,17 +2668,18 @@
         <v>79</v>
       </c>
       <c r="E64"/>
-      <c r="F64" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F64"/>
       <c r="G64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H64" s="1">
+      <c r="I64" s="1">
         <v>13782</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>38</v>
       </c>
@@ -2621,17 +2693,18 @@
         <v>104</v>
       </c>
       <c r="E65"/>
-      <c r="F65" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F65"/>
       <c r="G65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H65" s="1">
+      <c r="I65" s="1">
         <v>13682</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>98</v>
       </c>
@@ -2645,17 +2718,18 @@
         <v>76</v>
       </c>
       <c r="E66"/>
-      <c r="F66" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F66"/>
       <c r="G66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H66" s="1">
+      <c r="I66" s="1">
         <v>13644</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>28</v>
       </c>
@@ -2669,17 +2743,18 @@
         <v>105</v>
       </c>
       <c r="E67"/>
-      <c r="F67" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F67"/>
       <c r="G67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H67" s="1">
+      <c r="I67" s="1">
         <v>13618</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>125</v>
       </c>
@@ -2695,17 +2770,18 @@
       <c r="E68" t="s">
         <v>41</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68"/>
+      <c r="G68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="H68" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H68" s="1">
+      <c r="I68" s="1">
         <v>13613</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>95</v>
       </c>
@@ -2719,17 +2795,18 @@
         <v>107</v>
       </c>
       <c r="E69"/>
-      <c r="F69" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F69"/>
       <c r="G69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H69" s="1">
+      <c r="I69" s="1">
         <v>13504</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>135</v>
       </c>
@@ -2745,17 +2822,18 @@
       <c r="E70" t="s">
         <v>45</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70"/>
+      <c r="G70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="H70" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H70" s="1">
+      <c r="I70" s="1">
         <v>13461</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>65</v>
       </c>
@@ -2771,17 +2849,18 @@
       <c r="E71" t="s">
         <v>88</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F71"/>
       <c r="G71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H71" s="1">
+      <c r="I71" s="1">
         <v>13454</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>103</v>
       </c>
@@ -2795,17 +2874,18 @@
         <v>109</v>
       </c>
       <c r="E72"/>
-      <c r="F72" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F72"/>
       <c r="G72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="1">
+      <c r="I72" s="1">
         <v>13319</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>73</v>
       </c>
@@ -2819,17 +2899,18 @@
         <v>79</v>
       </c>
       <c r="E73"/>
-      <c r="F73" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F73"/>
       <c r="G73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H73" s="1">
+      <c r="I73" s="1">
         <v>13318</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>84</v>
       </c>
@@ -2843,17 +2924,18 @@
         <v>110</v>
       </c>
       <c r="E74"/>
-      <c r="F74" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F74"/>
       <c r="G74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H74" s="1">
+      <c r="I74" s="1">
         <v>13314</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>127</v>
       </c>
@@ -2866,20 +2948,20 @@
       <c r="D75" t="s">
         <v>75</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>83</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="H75" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H75" s="1">
+      <c r="I75" s="1">
         <v>13307</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>80</v>
       </c>
@@ -2893,17 +2975,18 @@
         <v>79</v>
       </c>
       <c r="E76"/>
-      <c r="F76" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F76"/>
       <c r="G76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H76" s="1">
+      <c r="I76" s="1">
         <v>13244</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>56</v>
       </c>
@@ -2916,20 +2999,20 @@
       <c r="D77" t="s">
         <v>112</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>83</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H77" s="1">
+      <c r="I77" s="1">
         <v>13219</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>57</v>
       </c>
@@ -2943,17 +3026,18 @@
         <v>113</v>
       </c>
       <c r="E78"/>
-      <c r="F78" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F78"/>
       <c r="G78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H78" s="1">
+      <c r="I78" s="1">
         <v>13140</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>62</v>
       </c>
@@ -2967,17 +3051,18 @@
         <v>81</v>
       </c>
       <c r="E79"/>
-      <c r="F79" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F79"/>
       <c r="G79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H79" s="1">
+      <c r="I79" s="1">
         <v>13085</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>31</v>
       </c>
@@ -2991,17 +3076,18 @@
         <v>114</v>
       </c>
       <c r="E80"/>
-      <c r="F80" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F80"/>
       <c r="G80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H80" s="1">
+      <c r="I80" s="1">
         <v>13074</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>52</v>
       </c>
@@ -3015,17 +3101,18 @@
         <v>115</v>
       </c>
       <c r="E81"/>
-      <c r="F81" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F81"/>
       <c r="G81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H81" s="1">
+      <c r="I81" s="1">
         <v>13019</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>136</v>
       </c>
@@ -3041,17 +3128,18 @@
       <c r="E82" t="s">
         <v>45</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82"/>
+      <c r="G82" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="H82" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H82" s="1">
+      <c r="I82" s="1">
         <v>12988</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>130</v>
       </c>
@@ -3064,20 +3152,20 @@
       <c r="D83" t="s">
         <v>117</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>83</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="G83" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="H83" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H83" s="1">
+      <c r="I83" s="1">
         <v>12940</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>107</v>
       </c>
@@ -3091,17 +3179,18 @@
         <v>118</v>
       </c>
       <c r="E84"/>
-      <c r="F84" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F84"/>
       <c r="G84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H84" s="1">
+      <c r="I84" s="1">
         <v>12922</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>82</v>
       </c>
@@ -3115,17 +3204,18 @@
         <v>119</v>
       </c>
       <c r="E85"/>
-      <c r="F85" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F85"/>
       <c r="G85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H85" s="1">
+      <c r="I85" s="1">
         <v>12840</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>79</v>
       </c>
@@ -3139,17 +3229,18 @@
         <v>79</v>
       </c>
       <c r="E86"/>
-      <c r="F86" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F86"/>
       <c r="G86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H86" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H86" s="1">
+      <c r="I86" s="1">
         <v>12777</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>42</v>
       </c>
@@ -3163,17 +3254,18 @@
         <v>77</v>
       </c>
       <c r="E87"/>
-      <c r="F87" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F87"/>
       <c r="G87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H87" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H87" s="1">
+      <c r="I87" s="1">
         <v>12707</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>101</v>
       </c>
@@ -3187,17 +3279,18 @@
         <v>76</v>
       </c>
       <c r="E88"/>
-      <c r="F88" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F88"/>
       <c r="G88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H88" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H88" s="1">
+      <c r="I88" s="1">
         <v>12540</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -3211,17 +3304,18 @@
         <v>110</v>
       </c>
       <c r="E89"/>
-      <c r="F89" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F89"/>
       <c r="G89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H89" s="1">
+      <c r="I89" s="1">
         <v>12495</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3235,17 +3329,18 @@
         <v>113</v>
       </c>
       <c r="E90"/>
-      <c r="F90" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F90"/>
       <c r="G90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H90" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H90" s="1">
+      <c r="I90" s="1">
         <v>12470</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>43</v>
       </c>
@@ -3259,17 +3354,18 @@
         <v>77</v>
       </c>
       <c r="E91"/>
-      <c r="F91" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F91"/>
       <c r="G91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H91" s="1">
+      <c r="I91" s="1">
         <v>12359</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>99</v>
       </c>
@@ -3283,17 +3379,18 @@
         <v>76</v>
       </c>
       <c r="E92"/>
-      <c r="F92" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F92"/>
       <c r="G92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H92" s="1">
+      <c r="I92" s="1">
         <v>12305</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>83</v>
       </c>
@@ -3307,17 +3404,18 @@
         <v>119</v>
       </c>
       <c r="E93"/>
-      <c r="F93" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F93"/>
       <c r="G93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H93" s="1">
+      <c r="I93" s="1">
         <v>12289</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>29</v>
       </c>
@@ -3331,17 +3429,18 @@
         <v>121</v>
       </c>
       <c r="E94"/>
-      <c r="F94" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F94"/>
       <c r="G94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H94" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H94" s="1">
+      <c r="I94" s="1">
         <v>12275</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -3355,17 +3454,18 @@
         <v>122</v>
       </c>
       <c r="E95"/>
-      <c r="F95" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F95"/>
       <c r="G95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H95" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H95" s="1">
+      <c r="I95" s="1">
         <v>12230</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>131</v>
       </c>
@@ -3378,20 +3478,20 @@
       <c r="D96" t="s">
         <v>117</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>83</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="G96" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G96" s="1" t="s">
+      <c r="H96" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H96" s="1">
+      <c r="I96" s="1">
         <v>12126</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>67</v>
       </c>
@@ -3407,17 +3507,18 @@
       <c r="E97" t="s">
         <v>66</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F97"/>
       <c r="G97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H97" s="1">
+      <c r="I97" s="1">
         <v>12000</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>105</v>
       </c>
@@ -3431,17 +3532,18 @@
         <v>109</v>
       </c>
       <c r="E98"/>
-      <c r="F98" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F98"/>
       <c r="G98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H98" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H98" s="1">
+      <c r="I98" s="1">
         <v>11989</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>30</v>
       </c>
@@ -3455,17 +3557,18 @@
         <v>123</v>
       </c>
       <c r="E99"/>
-      <c r="F99" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F99"/>
       <c r="G99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H99" s="1">
+      <c r="I99" s="1">
         <v>11932</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>19</v>
       </c>
@@ -3479,17 +3582,18 @@
         <v>124</v>
       </c>
       <c r="E100"/>
-      <c r="F100" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F100"/>
       <c r="G100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H100" s="1">
+      <c r="I100" s="1">
         <v>11900</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>47</v>
       </c>
@@ -3503,17 +3607,18 @@
         <v>125</v>
       </c>
       <c r="E101"/>
-      <c r="F101" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F101"/>
       <c r="G101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H101" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H101" s="1">
+      <c r="I101" s="1">
         <v>11868</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>61</v>
       </c>
@@ -3527,17 +3632,18 @@
         <v>81</v>
       </c>
       <c r="E102"/>
-      <c r="F102" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F102"/>
       <c r="G102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H102" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H102" s="1">
+      <c r="I102" s="1">
         <v>11689</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>106</v>
       </c>
@@ -3551,17 +3657,18 @@
         <v>126</v>
       </c>
       <c r="E103"/>
-      <c r="F103" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F103"/>
       <c r="G103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H103" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H103" s="1">
+      <c r="I103" s="1">
         <v>11596</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>44</v>
       </c>
@@ -3575,17 +3682,18 @@
         <v>127</v>
       </c>
       <c r="E104"/>
-      <c r="F104" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F104"/>
       <c r="G104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H104" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H104" s="1">
+      <c r="I104" s="1">
         <v>11453</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>10</v>
       </c>
@@ -3601,17 +3709,18 @@
       <c r="E105" t="s">
         <v>129</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F105"/>
       <c r="G105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H105" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H105" s="1">
+      <c r="I105" s="1">
         <v>11310</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>46</v>
       </c>
@@ -3625,17 +3734,18 @@
         <v>130</v>
       </c>
       <c r="E106"/>
-      <c r="F106" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F106"/>
       <c r="G106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H106" s="1">
+      <c r="I106" s="1">
         <v>11268</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>94</v>
       </c>
@@ -3649,17 +3759,18 @@
         <v>131</v>
       </c>
       <c r="E107"/>
-      <c r="F107" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F107"/>
       <c r="G107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H107" s="1">
+      <c r="I107" s="1">
         <v>11223</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>126</v>
       </c>
@@ -3672,20 +3783,20 @@
       <c r="D108" t="s">
         <v>132</v>
       </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>83</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="G108" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G108" s="1" t="s">
+      <c r="H108" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H108" s="1">
+      <c r="I108" s="1">
         <v>11215</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>11</v>
       </c>
@@ -3699,17 +3810,18 @@
         <v>133</v>
       </c>
       <c r="E109"/>
-      <c r="F109" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F109"/>
       <c r="G109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H109" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H109" s="1">
+      <c r="I109" s="1">
         <v>11149</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>33</v>
       </c>
@@ -3723,17 +3835,18 @@
         <v>114</v>
       </c>
       <c r="E110"/>
-      <c r="F110" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F110"/>
       <c r="G110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H110" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H110" s="1">
+      <c r="I110" s="1">
         <v>11100</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>53</v>
       </c>
@@ -3747,17 +3860,18 @@
         <v>134</v>
       </c>
       <c r="E111"/>
-      <c r="F111" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F111"/>
       <c r="G111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H111" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H111" s="1">
+      <c r="I111" s="1">
         <v>11047</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>115</v>
       </c>
@@ -3773,17 +3887,18 @@
       <c r="E112" t="s">
         <v>137</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="F112"/>
+      <c r="G112" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G112" s="1" t="s">
+      <c r="H112" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H112" s="1">
+      <c r="I112" s="1">
         <v>10956</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>32</v>
       </c>
@@ -3797,17 +3912,18 @@
         <v>114</v>
       </c>
       <c r="E113"/>
-      <c r="F113" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F113"/>
       <c r="G113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H113" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H113" s="1">
+      <c r="I113" s="1">
         <v>10955</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>7</v>
       </c>
@@ -3823,17 +3939,18 @@
       <c r="E114" t="s">
         <v>139</v>
       </c>
-      <c r="F114" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F114"/>
       <c r="G114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H114" s="1">
+      <c r="I114" s="1">
         <v>10900</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>39</v>
       </c>
@@ -3849,17 +3966,18 @@
       <c r="E115" t="s">
         <v>141</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F115"/>
       <c r="G115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H115" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H115" s="1">
+      <c r="I115" s="1">
         <v>10891</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>4</v>
       </c>
@@ -3873,17 +3991,18 @@
         <v>142</v>
       </c>
       <c r="E116"/>
-      <c r="F116" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F116"/>
       <c r="G116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H116" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H116" s="1">
+      <c r="I116" s="1">
         <v>10862</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>63</v>
       </c>
@@ -3897,17 +4016,18 @@
         <v>143</v>
       </c>
       <c r="E117"/>
-      <c r="F117" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F117"/>
       <c r="G117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H117" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H117" s="1">
+      <c r="I117" s="1">
         <v>10848</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>58</v>
       </c>
@@ -3921,17 +4041,18 @@
         <v>144</v>
       </c>
       <c r="E118"/>
-      <c r="F118" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F118"/>
       <c r="G118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H118" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H118" s="1">
+      <c r="I118" s="1">
         <v>10748</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>35</v>
       </c>
@@ -3945,17 +4066,18 @@
         <v>145</v>
       </c>
       <c r="E119"/>
-      <c r="F119" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F119"/>
       <c r="G119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H119" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H119" s="1">
+      <c r="I119" s="1">
         <v>10675</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>114</v>
       </c>
@@ -3971,17 +4093,18 @@
       <c r="E120" t="s">
         <v>137</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F120"/>
+      <c r="G120" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G120" s="1" t="s">
+      <c r="H120" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H120" s="1">
+      <c r="I120" s="1">
         <v>10672</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>134</v>
       </c>
@@ -3994,20 +4117,20 @@
       <c r="D121" t="s">
         <v>147</v>
       </c>
-      <c r="E121" t="s">
+      <c r="F121" t="s">
         <v>83</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="G121" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G121" s="1" t="s">
+      <c r="H121" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H121" s="1">
+      <c r="I121" s="1">
         <v>10593</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>14</v>
       </c>
@@ -4020,20 +4143,20 @@
       <c r="D122" t="s">
         <v>148</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>83</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H122" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H122" s="1">
+      <c r="I122" s="1">
         <v>10569</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>36</v>
       </c>
@@ -4047,17 +4170,18 @@
         <v>145</v>
       </c>
       <c r="E123"/>
-      <c r="F123" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F123"/>
       <c r="G123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H123" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H123" s="1">
+      <c r="I123" s="1">
         <v>10536</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>92</v>
       </c>
@@ -4071,17 +4195,18 @@
         <v>149</v>
       </c>
       <c r="E124"/>
-      <c r="F124" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F124"/>
       <c r="G124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H124" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H124" s="1">
+      <c r="I124" s="1">
         <v>10511</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>37</v>
       </c>
@@ -4095,17 +4220,18 @@
         <v>150</v>
       </c>
       <c r="E125"/>
-      <c r="F125" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F125"/>
       <c r="G125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H125" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H125" s="1">
+      <c r="I125" s="1">
         <v>10444</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>9</v>
       </c>
@@ -4121,17 +4247,18 @@
       <c r="E126" t="s">
         <v>129</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F126"/>
       <c r="G126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H126" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H126" s="1">
+      <c r="I126" s="1">
         <v>10424</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>133</v>
       </c>
@@ -4144,20 +4271,20 @@
       <c r="D127" t="s">
         <v>147</v>
       </c>
-      <c r="E127" t="s">
+      <c r="F127" t="s">
         <v>83</v>
       </c>
-      <c r="F127" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G127" s="1" t="s">
+      <c r="H127" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H127" s="1">
+      <c r="I127" s="1">
         <v>10397</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>129</v>
       </c>
@@ -4173,17 +4300,18 @@
       <c r="E128" t="s">
         <v>41</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F128"/>
+      <c r="G128" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G128" s="1" t="s">
+      <c r="H128" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H128" s="1">
+      <c r="I128" s="1">
         <v>10359</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>86</v>
       </c>
@@ -4197,17 +4325,18 @@
         <v>152</v>
       </c>
       <c r="E129"/>
-      <c r="F129" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F129"/>
       <c r="G129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H129" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H129" s="1">
+      <c r="I129" s="1">
         <v>10282</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>119</v>
       </c>
@@ -4223,17 +4352,18 @@
       <c r="E130" t="s">
         <v>155</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="F130"/>
+      <c r="G130" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="H130" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H130" s="1">
+      <c r="I130" s="1">
         <v>10103</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>116</v>
       </c>
@@ -4249,17 +4379,18 @@
       <c r="E131" t="s">
         <v>155</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F131"/>
+      <c r="G131" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="H131" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H131" s="1">
+      <c r="I131" s="1">
         <v>10071</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>117</v>
       </c>
@@ -4275,17 +4406,18 @@
       <c r="E132" t="s">
         <v>155</v>
       </c>
-      <c r="F132" s="1" t="s">
+      <c r="F132"/>
+      <c r="G132" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="H132" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H132" s="1">
+      <c r="I132" s="1">
         <v>9867</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>118</v>
       </c>
@@ -4301,17 +4433,18 @@
       <c r="E133" t="s">
         <v>155</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F133"/>
+      <c r="G133" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="H133" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H133" s="1">
+      <c r="I133" s="1">
         <v>9667</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>8</v>
       </c>
@@ -4327,17 +4460,18 @@
       <c r="E134" t="s">
         <v>139</v>
       </c>
-      <c r="F134" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F134"/>
       <c r="G134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H134" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H134" s="1">
+      <c r="I134" s="1">
         <v>6834</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>49</v>
       </c>
@@ -4353,17 +4487,18 @@
       <c r="E135" t="s">
         <v>158</v>
       </c>
-      <c r="F135" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F135"/>
       <c r="G135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H135" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H135" s="1">
+      <c r="I135" s="1">
         <v>5359</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>50</v>
       </c>
@@ -4379,17 +4514,18 @@
       <c r="E136" t="s">
         <v>158</v>
       </c>
-      <c r="F136" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F136"/>
       <c r="G136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H136" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H136" s="1">
+      <c r="I136" s="1">
         <v>5350</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>132</v>
       </c>
@@ -4405,13 +4541,14 @@
       <c r="E137" t="s">
         <v>160</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="F137"/>
+      <c r="G137" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G137" s="1" t="s">
+      <c r="H137" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H137" s="1">
+      <c r="I137" s="1">
         <v>4738</v>
       </c>
     </row>

</xml_diff>